<commit_message>
adding coordinator printouts (ongoing)
</commit_message>
<xml_diff>
--- a/config/security/little_register.xlsx
+++ b/config/security/little_register.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\adoration\config\security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0847694-E223-4E1E-B2DB-3C529E1BC333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6611D21-A967-46AA-97D3-9AC179EE7F26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{407EA927-167F-43C1-920F-BD0389F0FD15}"/>
   </bookViews>
@@ -448,19 +448,10 @@
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -470,18 +461,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -498,16 +504,10 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -962,7 +962,7 @@
   <dimension ref="B2:AD24"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,40 +978,40 @@
     <row r="2" spans="2:30" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="22"/>
+      <c r="AA2" s="22"/>
+      <c r="AB2" s="22"/>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
     <row r="3" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="2"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -1040,76 +1040,76 @@
       <c r="AD3" s="1"/>
     </row>
     <row r="4" spans="2:30" ht="61.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
-      <c r="AA4" s="5"/>
-      <c r="AB4" s="5"/>
-      <c r="AC4" s="5"/>
-      <c r="AD4" s="5"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="14"/>
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14"/>
     </row>
     <row r="5" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="6" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6"/>
-      <c r="AA5" s="6"/>
-      <c r="AB5" s="6"/>
-      <c r="AC5" s="7"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
+      <c r="X5" s="23"/>
+      <c r="Y5" s="23"/>
+      <c r="Z5" s="23"/>
+      <c r="AA5" s="23"/>
+      <c r="AB5" s="23"/>
+      <c r="AC5" s="4"/>
       <c r="AD5" s="1"/>
     </row>
     <row r="6" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="4"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -1137,109 +1137,109 @@
       <c r="AD6" s="1"/>
     </row>
     <row r="7" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="6"/>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="6"/>
-      <c r="AB7" s="6"/>
-      <c r="AC7" s="6"/>
-      <c r="AD7" s="6"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="23"/>
+      <c r="X7" s="23"/>
+      <c r="Y7" s="23"/>
+      <c r="Z7" s="23"/>
+      <c r="AA7" s="23"/>
+      <c r="AB7" s="23"/>
+      <c r="AC7" s="23"/>
+      <c r="AD7" s="23"/>
     </row>
     <row r="8" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="6"/>
-      <c r="AB8" s="6"/>
-      <c r="AC8" s="6"/>
-      <c r="AD8" s="6"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="23"/>
+      <c r="W8" s="23"/>
+      <c r="X8" s="23"/>
+      <c r="Y8" s="23"/>
+      <c r="Z8" s="23"/>
+      <c r="AA8" s="23"/>
+      <c r="AB8" s="23"/>
+      <c r="AC8" s="23"/>
+      <c r="AD8" s="23"/>
     </row>
     <row r="9" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="6" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="6"/>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="6"/>
-      <c r="Z9" s="6"/>
-      <c r="AA9" s="6"/>
-      <c r="AB9" s="6"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="23"/>
+      <c r="W9" s="23"/>
+      <c r="X9" s="23"/>
+      <c r="Y9" s="23"/>
+      <c r="Z9" s="23"/>
+      <c r="AA9" s="23"/>
+      <c r="AB9" s="23"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
     <row r="10" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1267,685 +1267,685 @@
       <c r="AD10" s="1"/>
     </row>
     <row r="11" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B11" s="4"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
-      <c r="V11" s="10"/>
-      <c r="W11" s="10"/>
-      <c r="X11" s="10"/>
-      <c r="Y11" s="10"/>
-      <c r="Z11" s="10"/>
-      <c r="AA11" s="10"/>
-      <c r="AB11" s="10"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="15"/>
+      <c r="AB11" s="15"/>
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
     </row>
     <row r="12" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="4"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="23">
+      <c r="B12" s="3"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="12">
         <v>0</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="12">
         <v>1</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="12">
         <v>2</v>
       </c>
-      <c r="H12" s="23">
+      <c r="H12" s="12">
         <v>3</v>
       </c>
-      <c r="I12" s="23">
+      <c r="I12" s="12">
         <v>4</v>
       </c>
-      <c r="J12" s="23">
+      <c r="J12" s="12">
         <v>5</v>
       </c>
-      <c r="K12" s="23">
+      <c r="K12" s="12">
         <v>6</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="7">
         <v>7</v>
       </c>
-      <c r="M12" s="11">
+      <c r="M12" s="7">
         <v>8</v>
       </c>
-      <c r="N12" s="11">
+      <c r="N12" s="7">
         <v>9</v>
       </c>
-      <c r="O12" s="11">
+      <c r="O12" s="7">
         <v>10</v>
       </c>
-      <c r="P12" s="11">
+      <c r="P12" s="7">
         <v>11</v>
       </c>
-      <c r="Q12" s="11">
+      <c r="Q12" s="7">
         <v>12</v>
       </c>
-      <c r="R12" s="11">
+      <c r="R12" s="7">
         <v>13</v>
       </c>
-      <c r="S12" s="11">
+      <c r="S12" s="7">
         <v>14</v>
       </c>
-      <c r="T12" s="11">
+      <c r="T12" s="7">
         <v>15</v>
       </c>
-      <c r="U12" s="11">
+      <c r="U12" s="7">
         <v>16</v>
       </c>
-      <c r="V12" s="11">
+      <c r="V12" s="7">
         <v>17</v>
       </c>
-      <c r="W12" s="11">
+      <c r="W12" s="7">
         <v>18</v>
       </c>
-      <c r="X12" s="11">
+      <c r="X12" s="7">
         <v>19</v>
       </c>
-      <c r="Y12" s="23">
+      <c r="Y12" s="12">
         <v>20</v>
       </c>
-      <c r="Z12" s="23">
+      <c r="Z12" s="12">
         <v>21</v>
       </c>
-      <c r="AA12" s="23">
+      <c r="AA12" s="12">
         <v>22</v>
       </c>
-      <c r="AB12" s="23">
+      <c r="AB12" s="12">
         <v>23</v>
       </c>
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
     </row>
     <row r="13" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B13" s="4"/>
-      <c r="C13" s="12" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="14" t="str">
-        <f t="shared" ref="F13:AB19" si="0">IF(L40="","",IF(L40&gt;1,"❷","①"))</f>
-        <v/>
-      </c>
-      <c r="M13" s="14" t="str">
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="9" t="str">
+        <f>IF(L40=0,"",IF(L40&gt;1,"❷","①"))</f>
+        <v/>
+      </c>
+      <c r="M13" s="9" t="str">
+        <f t="shared" ref="M13:X13" si="0">IF(M40=0,"",IF(M40&gt;1,"❷","①"))</f>
+        <v/>
+      </c>
+      <c r="N13" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="N13" s="14" t="str">
+      <c r="O13" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="O13" s="14" t="str">
+      <c r="P13" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P13" s="14" t="str">
+      <c r="Q13" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="Q13" s="14" t="str">
+      <c r="R13" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="R13" s="14" t="str">
+      <c r="S13" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S13" s="14" t="str">
+      <c r="T13" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="T13" s="14" t="str">
+      <c r="U13" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="U13" s="14" t="str">
+      <c r="V13" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="V13" s="14" t="str">
+      <c r="W13" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="W13" s="14" t="str">
+      <c r="X13" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="X13" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Y13" s="22"/>
-      <c r="Z13" s="22"/>
-      <c r="AA13" s="22"/>
-      <c r="AB13" s="22"/>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="11"/>
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
     </row>
     <row r="14" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B14" s="4"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="14" t="str">
-        <f t="shared" ref="E14:T19" si="1">IF(L41="","",IF(L41&gt;1,"❷","①"))</f>
-        <v/>
-      </c>
-      <c r="M14" s="14" t="str">
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="9" t="str">
+        <f t="shared" ref="L14:X14" si="1">IF(L41=0,"",IF(L41&gt;1,"❷","①"))</f>
+        <v/>
+      </c>
+      <c r="M14" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N14" s="14" t="str">
+      <c r="N14" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="O14" s="14" t="str">
+      <c r="O14" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P14" s="14" t="str">
+      <c r="P14" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="Q14" s="14" t="str">
+      <c r="Q14" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="R14" s="14" t="str">
+      <c r="R14" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="S14" s="14" t="str">
+      <c r="S14" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="T14" s="14" t="str">
+      <c r="T14" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U14" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="V14" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="W14" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X14" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Y14" s="22"/>
-      <c r="Z14" s="22"/>
-      <c r="AA14" s="22"/>
-      <c r="AB14" s="22"/>
+      <c r="U14" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="V14" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="W14" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="X14" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="11"/>
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
     </row>
     <row r="15" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B15" s="4"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13" t="s">
+      <c r="B15" s="3"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M15" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N15" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O15" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="P15" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q15" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="R15" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="S15" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="T15" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="U15" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="V15" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="W15" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X15" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Y15" s="22"/>
-      <c r="Z15" s="22"/>
-      <c r="AA15" s="22"/>
-      <c r="AB15" s="22"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="9" t="str">
+        <f t="shared" ref="L15:X15" si="2">IF(L42=0,"",IF(L42&gt;1,"❷","①"))</f>
+        <v/>
+      </c>
+      <c r="M15" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N15" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="O15" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="P15" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="Q15" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="R15" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S15" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="T15" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="U15" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="V15" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="W15" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="X15" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="11"/>
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
     </row>
     <row r="16" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B16" s="4"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="13" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M16" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N16" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O16" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="P16" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q16" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="R16" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="S16" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="T16" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="U16" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="V16" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="W16" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X16" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Y16" s="22"/>
-      <c r="Z16" s="22"/>
-      <c r="AA16" s="22"/>
-      <c r="AB16" s="22"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="9" t="str">
+        <f t="shared" ref="L16:X16" si="3">IF(L43=0,"",IF(L43&gt;1,"❷","①"))</f>
+        <v/>
+      </c>
+      <c r="M16" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="N16" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="O16" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="P16" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="Q16" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="R16" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="S16" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="T16" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="U16" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="V16" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="W16" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="X16" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="11"/>
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
     </row>
     <row r="17" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B17" s="4"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="13" t="s">
+      <c r="B17" s="3"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M17" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N17" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O17" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="P17" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q17" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="R17" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="S17" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="T17" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="U17" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="V17" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="W17" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X17" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Y17" s="22"/>
-      <c r="Z17" s="22"/>
-      <c r="AA17" s="22"/>
-      <c r="AB17" s="22"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="9" t="str">
+        <f t="shared" ref="L17:X17" si="4">IF(L44=0,"",IF(L44&gt;1,"❷","①"))</f>
+        <v/>
+      </c>
+      <c r="M17" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="N17" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="O17" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="P17" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Q17" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R17" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S17" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="T17" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="U17" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="V17" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="W17" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="X17" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="11"/>
+      <c r="AA17" s="11"/>
+      <c r="AB17" s="11"/>
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
     </row>
     <row r="18" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B18" s="4"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13" t="s">
+      <c r="B18" s="3"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M18" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N18" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O18" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="P18" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q18" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="R18" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="S18" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="T18" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="U18" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="V18" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="W18" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X18" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Y18" s="22"/>
-      <c r="Z18" s="22"/>
-      <c r="AA18" s="22"/>
-      <c r="AB18" s="22"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="9" t="str">
+        <f t="shared" ref="L18:X18" si="5">IF(L45=0,"",IF(L45&gt;1,"❷","①"))</f>
+        <v/>
+      </c>
+      <c r="M18" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N18" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O18" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="P18" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Q18" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="R18" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="S18" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="T18" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="U18" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="V18" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="W18" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X18" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="11"/>
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
     </row>
     <row r="19" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B19" s="4"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13" t="s">
+      <c r="B19" s="3"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M19" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N19" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O19" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="P19" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q19" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="R19" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="S19" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="T19" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="U19" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="V19" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="W19" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X19" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Y19" s="22"/>
-      <c r="Z19" s="22"/>
-      <c r="AA19" s="22"/>
-      <c r="AB19" s="22"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="9" t="str">
+        <f t="shared" ref="L19:X19" si="6">IF(L46=0,"",IF(L46&gt;1,"❷","①"))</f>
+        <v/>
+      </c>
+      <c r="M19" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="N19" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="O19" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="P19" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q19" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="R19" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="S19" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="T19" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="U19" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="V19" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="W19" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="X19" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="11"/>
       <c r="AC19" s="1"/>
       <c r="AD19" s="1"/>
     </row>
     <row r="20" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B20" s="4"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="15" t="s">
+      <c r="B20" s="3"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="10" t="s">
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="15" t="s">
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="10"/>
-      <c r="V20" s="16"/>
-      <c r="W20" s="17" t="s">
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="18"/>
+      <c r="W20" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="X20" s="18"/>
-      <c r="Y20" s="18"/>
-      <c r="Z20" s="18"/>
-      <c r="AA20" s="18"/>
-      <c r="AB20" s="19"/>
+      <c r="X20" s="20"/>
+      <c r="Y20" s="20"/>
+      <c r="Z20" s="20"/>
+      <c r="AA20" s="20"/>
+      <c r="AB20" s="21"/>
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
     </row>
     <row r="21" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
@@ -1955,75 +1955,75 @@
       <c r="AD21" s="1"/>
     </row>
     <row r="22" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="21"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="21"/>
-      <c r="U22" s="21"/>
-      <c r="V22" s="21"/>
-      <c r="W22" s="21"/>
-      <c r="X22" s="21"/>
-      <c r="Y22" s="21"/>
-      <c r="Z22" s="21"/>
-      <c r="AA22" s="21"/>
-      <c r="AB22" s="21"/>
-      <c r="AC22" s="21"/>
-      <c r="AD22" s="21"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="13"/>
+      <c r="W22" s="13"/>
+      <c r="X22" s="13"/>
+      <c r="Y22" s="13"/>
+      <c r="Z22" s="13"/>
+      <c r="AA22" s="13"/>
+      <c r="AB22" s="13"/>
+      <c r="AC22" s="13"/>
+      <c r="AD22" s="13"/>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="21" t="s">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="21"/>
-      <c r="L23" s="21"/>
-      <c r="M23" s="21"/>
-      <c r="N23" s="21"/>
-      <c r="O23" s="21"/>
-      <c r="P23" s="21"/>
-      <c r="Q23" s="21"/>
-      <c r="R23" s="21"/>
-      <c r="S23" s="21"/>
-      <c r="T23" s="21"/>
-      <c r="U23" s="21"/>
-      <c r="V23" s="21"/>
-      <c r="W23" s="21"/>
-      <c r="X23" s="21"/>
-      <c r="Y23" s="21"/>
-      <c r="Z23" s="21"/>
-      <c r="AA23" s="21"/>
-      <c r="AB23" s="21"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
+      <c r="T23" s="13"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="13"/>
+      <c r="W23" s="13"/>
+      <c r="X23" s="13"/>
+      <c r="Y23" s="13"/>
+      <c r="Z23" s="13"/>
+      <c r="AA23" s="13"/>
+      <c r="AB23" s="13"/>
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
     </row>
     <row r="24" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="2"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -2053,6 +2053,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D2:AB2"/>
+    <mergeCell ref="D5:AB5"/>
+    <mergeCell ref="B7:AD7"/>
+    <mergeCell ref="B8:AD8"/>
+    <mergeCell ref="D9:AB9"/>
     <mergeCell ref="D23:AB23"/>
     <mergeCell ref="B4:AD4"/>
     <mergeCell ref="B22:AD22"/>
@@ -2062,11 +2067,6 @@
     <mergeCell ref="K20:P20"/>
     <mergeCell ref="Q20:V20"/>
     <mergeCell ref="W20:AB20"/>
-    <mergeCell ref="D2:AB2"/>
-    <mergeCell ref="D5:AB5"/>
-    <mergeCell ref="B7:AD7"/>
-    <mergeCell ref="B8:AD8"/>
-    <mergeCell ref="D9:AB9"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:AB19">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
ui update at information page
</commit_message>
<xml_diff>
--- a/config/security/little_register.xlsx
+++ b/config/security/little_register.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\adoration\config\security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6611D21-A967-46AA-97D3-9AC179EE7F26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF773502-6D77-4F23-A36A-F41F64209933}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{407EA927-167F-43C1-920F-BD0389F0FD15}"/>
+    <workbookView xWindow="3555" yWindow="1170" windowWidth="24585" windowHeight="11385" xr2:uid="{407EA927-167F-43C1-920F-BD0389F0FD15}"/>
   </bookViews>
   <sheets>
     <sheet name="Adorálók" sheetId="1" r:id="rId1"/>
@@ -477,6 +477,12 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -503,12 +509,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -876,7 +876,7 @@
   <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,8 +961,8 @@
   </sheetPr>
   <dimension ref="B2:AD24"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,33 +978,33 @@
     <row r="2" spans="2:30" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="22"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="13"/>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
@@ -1040,68 +1040,68 @@
       <c r="AD3" s="1"/>
     </row>
     <row r="4" spans="2:30" ht="61.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
-      <c r="W4" s="14"/>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="14"/>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="14"/>
-      <c r="AB4" s="14"/>
-      <c r="AC4" s="14"/>
-      <c r="AD4" s="14"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="16"/>
+      <c r="AB4" s="16"/>
+      <c r="AC4" s="16"/>
+      <c r="AD4" s="16"/>
     </row>
     <row r="5" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="23"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="23"/>
-      <c r="X5" s="23"/>
-      <c r="Y5" s="23"/>
-      <c r="Z5" s="23"/>
-      <c r="AA5" s="23"/>
-      <c r="AB5" s="23"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="14"/>
+      <c r="AB5" s="14"/>
       <c r="AC5" s="4"/>
       <c r="AD5" s="1"/>
     </row>
@@ -1137,101 +1137,101 @@
       <c r="AD6" s="1"/>
     </row>
     <row r="7" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="23"/>
-      <c r="W7" s="23"/>
-      <c r="X7" s="23"/>
-      <c r="Y7" s="23"/>
-      <c r="Z7" s="23"/>
-      <c r="AA7" s="23"/>
-      <c r="AB7" s="23"/>
-      <c r="AC7" s="23"/>
-      <c r="AD7" s="23"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="14"/>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="14"/>
+      <c r="Z7" s="14"/>
+      <c r="AA7" s="14"/>
+      <c r="AB7" s="14"/>
+      <c r="AC7" s="14"/>
+      <c r="AD7" s="14"/>
     </row>
     <row r="8" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="23"/>
-      <c r="V8" s="23"/>
-      <c r="W8" s="23"/>
-      <c r="X8" s="23"/>
-      <c r="Y8" s="23"/>
-      <c r="Z8" s="23"/>
-      <c r="AA8" s="23"/>
-      <c r="AB8" s="23"/>
-      <c r="AC8" s="23"/>
-      <c r="AD8" s="23"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="14"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="14"/>
+      <c r="AB8" s="14"/>
+      <c r="AC8" s="14"/>
+      <c r="AD8" s="14"/>
     </row>
     <row r="9" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="23"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="23"/>
-      <c r="X9" s="23"/>
-      <c r="Y9" s="23"/>
-      <c r="Z9" s="23"/>
-      <c r="AA9" s="23"/>
-      <c r="AB9" s="23"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="14"/>
+      <c r="Z9" s="14"/>
+      <c r="AA9" s="14"/>
+      <c r="AB9" s="14"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
@@ -1270,32 +1270,32 @@
       <c r="B11" s="3"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="15"/>
-      <c r="AA11" s="15"/>
-      <c r="AB11" s="15"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="17"/>
+      <c r="Y11" s="17"/>
+      <c r="Z11" s="17"/>
+      <c r="AA11" s="17"/>
+      <c r="AB11" s="17"/>
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
     </row>
@@ -1380,7 +1380,7 @@
     </row>
     <row r="13" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="18" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="8" t="s">
@@ -1454,9 +1454,9 @@
     </row>
     <row r="14" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
-      <c r="C14" s="16"/>
+      <c r="C14" s="18"/>
       <c r="D14" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -1526,9 +1526,9 @@
     </row>
     <row r="15" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
-      <c r="C15" s="16"/>
+      <c r="C15" s="18"/>
       <c r="D15" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
@@ -1598,9 +1598,9 @@
     </row>
     <row r="16" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
-      <c r="C16" s="16"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
@@ -1670,9 +1670,9 @@
     </row>
     <row r="17" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
-      <c r="C17" s="16"/>
+      <c r="C17" s="18"/>
       <c r="D17" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
@@ -1742,9 +1742,9 @@
     </row>
     <row r="18" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
-      <c r="C18" s="16"/>
+      <c r="C18" s="18"/>
       <c r="D18" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
@@ -1814,9 +1814,9 @@
     </row>
     <row r="19" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
-      <c r="C19" s="16"/>
+      <c r="C19" s="18"/>
       <c r="D19" s="8" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
@@ -1888,38 +1888,38 @@
       <c r="B20" s="3"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="15" t="s">
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="17" t="s">
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="R20" s="15"/>
-      <c r="S20" s="15"/>
-      <c r="T20" s="15"/>
-      <c r="U20" s="15"/>
-      <c r="V20" s="18"/>
-      <c r="W20" s="19" t="s">
+      <c r="R20" s="17"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="17"/>
+      <c r="U20" s="17"/>
+      <c r="V20" s="20"/>
+      <c r="W20" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="X20" s="20"/>
-      <c r="Y20" s="20"/>
-      <c r="Z20" s="20"/>
-      <c r="AA20" s="20"/>
-      <c r="AB20" s="21"/>
+      <c r="X20" s="22"/>
+      <c r="Y20" s="22"/>
+      <c r="Z20" s="22"/>
+      <c r="AA20" s="22"/>
+      <c r="AB20" s="23"/>
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
     </row>
@@ -1955,68 +1955,68 @@
       <c r="AD21" s="1"/>
     </row>
     <row r="22" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13"/>
-      <c r="U22" s="13"/>
-      <c r="V22" s="13"/>
-      <c r="W22" s="13"/>
-      <c r="X22" s="13"/>
-      <c r="Y22" s="13"/>
-      <c r="Z22" s="13"/>
-      <c r="AA22" s="13"/>
-      <c r="AB22" s="13"/>
-      <c r="AC22" s="13"/>
-      <c r="AD22" s="13"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="15"/>
+      <c r="W22" s="15"/>
+      <c r="X22" s="15"/>
+      <c r="Y22" s="15"/>
+      <c r="Z22" s="15"/>
+      <c r="AA22" s="15"/>
+      <c r="AB22" s="15"/>
+      <c r="AC22" s="15"/>
+      <c r="AD22" s="15"/>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
-      <c r="T23" s="13"/>
-      <c r="U23" s="13"/>
-      <c r="V23" s="13"/>
-      <c r="W23" s="13"/>
-      <c r="X23" s="13"/>
-      <c r="Y23" s="13"/>
-      <c r="Z23" s="13"/>
-      <c r="AA23" s="13"/>
-      <c r="AB23" s="13"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="15"/>
+      <c r="U23" s="15"/>
+      <c r="V23" s="15"/>
+      <c r="W23" s="15"/>
+      <c r="X23" s="15"/>
+      <c r="Y23" s="15"/>
+      <c r="Z23" s="15"/>
+      <c r="AA23" s="15"/>
+      <c r="AB23" s="15"/>
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
     </row>
@@ -2053,11 +2053,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D2:AB2"/>
-    <mergeCell ref="D5:AB5"/>
-    <mergeCell ref="B7:AD7"/>
-    <mergeCell ref="B8:AD8"/>
-    <mergeCell ref="D9:AB9"/>
     <mergeCell ref="D23:AB23"/>
     <mergeCell ref="B4:AD4"/>
     <mergeCell ref="B22:AD22"/>
@@ -2067,6 +2062,11 @@
     <mergeCell ref="K20:P20"/>
     <mergeCell ref="Q20:V20"/>
     <mergeCell ref="W20:AB20"/>
+    <mergeCell ref="D2:AB2"/>
+    <mergeCell ref="D5:AB5"/>
+    <mergeCell ref="B7:AD7"/>
+    <mergeCell ref="B8:AD8"/>
+    <mergeCell ref="D9:AB9"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:AB19">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
- fix coverage printing in xls - show hour-coordinators on Information page - other minor updates
</commit_message>
<xml_diff>
--- a/config/security/little_register.xlsx
+++ b/config/security/little_register.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\adoration\config\security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF773502-6D77-4F23-A36A-F41F64209933}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05552CFA-68EA-4E43-8C20-FC9E8B6BBDF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="1170" windowWidth="24585" windowHeight="11385" xr2:uid="{407EA927-167F-43C1-920F-BD0389F0FD15}"/>
+    <workbookView xWindow="3015" yWindow="1860" windowWidth="24975" windowHeight="12300" activeTab="1" xr2:uid="{407EA927-167F-43C1-920F-BD0389F0FD15}"/>
   </bookViews>
   <sheets>
     <sheet name="Adorálók" sheetId="1" r:id="rId1"/>
@@ -85,6 +85,51 @@
     <t>Folyamatosan keresünk szentségimádókat!</t>
   </si>
   <si>
+    <t>és azt dobd be a piarista rendház postaládájába, vagy egyszerűen hagyd bent a kápolnában egy jól látható helyen</t>
+  </si>
+  <si>
+    <t>Órák</t>
+  </si>
+  <si>
+    <t>Napok</t>
+  </si>
+  <si>
+    <t>Hétfő</t>
+  </si>
+  <si>
+    <t>Kedd</t>
+  </si>
+  <si>
+    <t>Szerda</t>
+  </si>
+  <si>
+    <t>Csütörtök</t>
+  </si>
+  <si>
+    <t>Péntek</t>
+  </si>
+  <si>
+    <t>Szombat</t>
+  </si>
+  <si>
+    <t>Vasárnap</t>
+  </si>
+  <si>
+    <t>Hajnal</t>
+  </si>
+  <si>
+    <t>Délelőtt</t>
+  </si>
+  <si>
+    <t>Délután</t>
+  </si>
+  <si>
+    <t>Este</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aki jelenleg rendszeres szentségimádást végez egy adott órában, és az az óra a táblázatban 1-gyel van jelölve, az ne jelentkezzen át máshova, hiszen csak egyedül van az adott órában. </t>
+  </si>
+  <si>
     <r>
       <t>elsősorban a lenti táblázatban</t>
     </r>
@@ -96,17 +141,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> 2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="20"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>-ve</t>
+      <t xml:space="preserve"> 2-ve</t>
     </r>
     <r>
       <rPr>
@@ -117,7 +152,16 @@
         <family val="2"/>
         <charset val="238"/>
       </rPr>
-      <t>l és 1-gyel jelölt</t>
+      <t>l jelölt órákra</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, illetve másodsorban az 1-gyel jelölt</t>
     </r>
     <r>
       <rPr>
@@ -127,7 +171,7 @@
         <family val="2"/>
         <charset val="238"/>
       </rPr>
-      <t xml:space="preserve"> napokra és órákra.</t>
+      <t xml:space="preserve"> órákra.</t>
     </r>
   </si>
   <si>
@@ -142,7 +186,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> kérlek töltsd ki a mellékelt jelentkezési lapot</t>
+      <t xml:space="preserve"> kérlek töltsd ki a jelentkezési lapot</t>
     </r>
     <r>
       <rPr>
@@ -156,9 +200,6 @@
     </r>
   </si>
   <si>
-    <t>és azt dobd be a piarista rendház postaládájába, vagy egyszerűen hagyd bent a kápolnában egy jól látható helyen</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">vagy jelentkezz a </t>
     </r>
@@ -170,7 +211,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>https://orokimadas.info/vac</t>
+      <t>https://orokimadas.info</t>
     </r>
     <r>
       <rPr>
@@ -184,48 +225,6 @@
     </r>
   </si>
   <si>
-    <t>Órák</t>
-  </si>
-  <si>
-    <t>Napok</t>
-  </si>
-  <si>
-    <t>Hétfő</t>
-  </si>
-  <si>
-    <t>Kedd</t>
-  </si>
-  <si>
-    <t>Szerda</t>
-  </si>
-  <si>
-    <t>Csütörtök</t>
-  </si>
-  <si>
-    <t>Péntek</t>
-  </si>
-  <si>
-    <t>Szombat</t>
-  </si>
-  <si>
-    <t>Vasárnap</t>
-  </si>
-  <si>
-    <t>Hajnal</t>
-  </si>
-  <si>
-    <t>Délelőtt</t>
-  </si>
-  <si>
-    <t>Délután</t>
-  </si>
-  <si>
-    <t>Este</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aki jelenleg rendszeres szentségimádást végez egy adott órában, és az az óra a táblázatban 1-gyel van jelölve, az ne jelentkezzen át máshova, hiszen csak egyedül van az adott órában. </t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">További információk: </t>
     </r>
@@ -237,7 +236,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>https://orokimadas.info/vac</t>
+      <t>https://orokimadas.info</t>
     </r>
   </si>
 </sst>
@@ -245,7 +244,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,6 +317,12 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -445,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -453,9 +458,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -475,12 +477,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -510,6 +506,12 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,15 +534,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>116416</xdr:colOff>
+      <xdr:colOff>508000</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>124884</xdr:rowOff>
+      <xdr:rowOff>93135</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1573741</xdr:colOff>
+      <xdr:colOff>1965325</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>158640</xdr:rowOff>
+      <xdr:rowOff>126891</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -563,7 +565,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="730249" y="4061884"/>
+          <a:off x="1121833" y="4030135"/>
           <a:ext cx="1457325" cy="1494256"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -875,7 +877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA08CD39-1EF9-4B66-A21C-E44C706C1B79}">
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -961,50 +963,50 @@
   </sheetPr>
   <dimension ref="B2:AD24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AG30" sqref="AG30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
     <col min="5" max="28" width="5.140625" customWidth="1"/>
-    <col min="29" max="29" width="10" customWidth="1"/>
+    <col min="29" max="29" width="6.85546875" customWidth="1"/>
     <col min="30" max="30" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:30" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="13"/>
-      <c r="X2" s="13"/>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13"/>
-      <c r="AA2" s="13"/>
-      <c r="AB2" s="13"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="21"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="21"/>
+      <c r="AB2" s="21"/>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
@@ -1040,75 +1042,75 @@
       <c r="AD3" s="1"/>
     </row>
     <row r="4" spans="2:30" ht="61.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="16"/>
-      <c r="AA4" s="16"/>
-      <c r="AB4" s="16"/>
-      <c r="AC4" s="16"/>
-      <c r="AD4" s="16"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="13"/>
+      <c r="V4" s="13"/>
+      <c r="W4" s="13"/>
+      <c r="X4" s="13"/>
+      <c r="Y4" s="13"/>
+      <c r="Z4" s="13"/>
+      <c r="AA4" s="13"/>
+      <c r="AB4" s="13"/>
+      <c r="AC4" s="13"/>
+      <c r="AD4" s="13"/>
     </row>
     <row r="5" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14"/>
-      <c r="W5" s="14"/>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="14"/>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="14"/>
-      <c r="AB5" s="14"/>
-      <c r="AC5" s="4"/>
-      <c r="AD5" s="1"/>
+      <c r="B5" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="22"/>
+      <c r="W5" s="22"/>
+      <c r="X5" s="22"/>
+      <c r="Y5" s="22"/>
+      <c r="Z5" s="22"/>
+      <c r="AA5" s="22"/>
+      <c r="AB5" s="22"/>
+      <c r="AC5" s="22"/>
+      <c r="AD5" s="22"/>
     </row>
     <row r="6" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="5"/>
+      <c r="D6" s="4"/>
       <c r="E6" s="3"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -1137,101 +1139,101 @@
       <c r="AD6" s="1"/>
     </row>
     <row r="7" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="14"/>
-      <c r="V7" s="14"/>
-      <c r="W7" s="14"/>
-      <c r="X7" s="14"/>
-      <c r="Y7" s="14"/>
-      <c r="Z7" s="14"/>
-      <c r="AA7" s="14"/>
-      <c r="AB7" s="14"/>
-      <c r="AC7" s="14"/>
-      <c r="AD7" s="14"/>
+      <c r="B7" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="22"/>
+      <c r="W7" s="22"/>
+      <c r="X7" s="22"/>
+      <c r="Y7" s="22"/>
+      <c r="Z7" s="22"/>
+      <c r="AA7" s="22"/>
+      <c r="AB7" s="22"/>
+      <c r="AC7" s="22"/>
+      <c r="AD7" s="22"/>
     </row>
     <row r="8" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="14"/>
-      <c r="W8" s="14"/>
-      <c r="X8" s="14"/>
-      <c r="Y8" s="14"/>
-      <c r="Z8" s="14"/>
-      <c r="AA8" s="14"/>
-      <c r="AB8" s="14"/>
-      <c r="AC8" s="14"/>
-      <c r="AD8" s="14"/>
+      <c r="B8" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="22"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="22"/>
+      <c r="U8" s="22"/>
+      <c r="V8" s="22"/>
+      <c r="W8" s="22"/>
+      <c r="X8" s="22"/>
+      <c r="Y8" s="22"/>
+      <c r="Z8" s="22"/>
+      <c r="AA8" s="22"/>
+      <c r="AB8" s="22"/>
+      <c r="AC8" s="22"/>
+      <c r="AD8" s="22"/>
     </row>
     <row r="9" spans="2:30" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="14"/>
-      <c r="W9" s="14"/>
-      <c r="X9" s="14"/>
-      <c r="Y9" s="14"/>
-      <c r="Z9" s="14"/>
-      <c r="AA9" s="14"/>
-      <c r="AB9" s="14"/>
+      <c r="D9" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="22"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
@@ -1268,111 +1270,111 @@
     </row>
     <row r="11" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="17"/>
-      <c r="V11" s="17"/>
-      <c r="W11" s="17"/>
-      <c r="X11" s="17"/>
-      <c r="Y11" s="17"/>
-      <c r="Z11" s="17"/>
-      <c r="AA11" s="17"/>
-      <c r="AB11" s="17"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="14"/>
+      <c r="AA11" s="14"/>
+      <c r="AB11" s="14"/>
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
     </row>
     <row r="12" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="12">
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="11">
         <v>0</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="11">
         <v>1</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="11">
         <v>2</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="11">
         <v>3</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="11">
         <v>4</v>
       </c>
-      <c r="J12" s="12">
+      <c r="J12" s="11">
         <v>5</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K12" s="11">
         <v>6</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="6">
         <v>7</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="6">
         <v>8</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N12" s="6">
         <v>9</v>
       </c>
-      <c r="O12" s="7">
+      <c r="O12" s="6">
         <v>10</v>
       </c>
-      <c r="P12" s="7">
+      <c r="P12" s="6">
         <v>11</v>
       </c>
-      <c r="Q12" s="7">
+      <c r="Q12" s="6">
         <v>12</v>
       </c>
-      <c r="R12" s="7">
+      <c r="R12" s="6">
         <v>13</v>
       </c>
-      <c r="S12" s="7">
+      <c r="S12" s="6">
         <v>14</v>
       </c>
-      <c r="T12" s="7">
+      <c r="T12" s="6">
         <v>15</v>
       </c>
-      <c r="U12" s="7">
+      <c r="U12" s="6">
         <v>16</v>
       </c>
-      <c r="V12" s="7">
+      <c r="V12" s="6">
         <v>17</v>
       </c>
-      <c r="W12" s="7">
+      <c r="W12" s="6">
         <v>18</v>
       </c>
-      <c r="X12" s="7">
+      <c r="X12" s="11">
         <v>19</v>
       </c>
-      <c r="Y12" s="12">
+      <c r="Y12" s="11">
         <v>20</v>
       </c>
-      <c r="Z12" s="12">
+      <c r="Z12" s="11">
         <v>21</v>
       </c>
-      <c r="AA12" s="12">
+      <c r="AA12" s="11">
         <v>22</v>
       </c>
-      <c r="AB12" s="12">
+      <c r="AB12" s="11">
         <v>23</v>
       </c>
       <c r="AC12" s="1"/>
@@ -1380,553 +1382,532 @@
     </row>
     <row r="13" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
-      <c r="C13" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="9" t="str">
+      <c r="C13" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="8" t="str">
         <f>IF(L40=0,"",IF(L40&gt;1,"❷","①"))</f>
         <v/>
       </c>
-      <c r="M13" s="9" t="str">
-        <f t="shared" ref="M13:X13" si="0">IF(M40=0,"",IF(M40&gt;1,"❷","①"))</f>
-        <v/>
-      </c>
-      <c r="N13" s="9" t="str">
+      <c r="M13" s="8" t="str">
+        <f t="shared" ref="M13:W13" si="0">IF(M40=0,"",IF(M40&gt;1,"❷","①"))</f>
+        <v/>
+      </c>
+      <c r="N13" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="O13" s="9" t="str">
+      <c r="O13" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P13" s="9" t="str">
+      <c r="P13" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="Q13" s="9" t="str">
+      <c r="Q13" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="R13" s="9" t="str">
+      <c r="R13" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S13" s="9" t="str">
+      <c r="S13" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="T13" s="9" t="str">
+      <c r="T13" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="U13" s="9" t="str">
+      <c r="U13" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="V13" s="9" t="str">
+      <c r="V13" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="W13" s="9" t="str">
+      <c r="W13" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="X13" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Y13" s="11"/>
-      <c r="Z13" s="11"/>
-      <c r="AA13" s="11"/>
-      <c r="AB13" s="11"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="10"/>
+      <c r="AA13" s="10"/>
+      <c r="AB13" s="10"/>
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
     </row>
     <row r="14" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="9" t="str">
-        <f t="shared" ref="L14:X14" si="1">IF(L41=0,"",IF(L41&gt;1,"❷","①"))</f>
-        <v/>
-      </c>
-      <c r="M14" s="9" t="str">
+      <c r="C14" s="15"/>
+      <c r="D14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="8" t="str">
+        <f t="shared" ref="L14:W14" si="1">IF(L41=0,"",IF(L41&gt;1,"❷","①"))</f>
+        <v/>
+      </c>
+      <c r="M14" s="8" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N14" s="9" t="str">
+      <c r="N14" s="8" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="O14" s="9" t="str">
+      <c r="O14" s="8" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="P14" s="9" t="str">
+      <c r="P14" s="8" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="Q14" s="9" t="str">
+      <c r="Q14" s="8" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="R14" s="9" t="str">
+      <c r="R14" s="8" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="S14" s="9" t="str">
+      <c r="S14" s="8" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="T14" s="9" t="str">
+      <c r="T14" s="8" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="U14" s="9" t="str">
+      <c r="U14" s="8" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="V14" s="9" t="str">
+      <c r="V14" s="8" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="W14" s="9" t="str">
+      <c r="W14" s="8" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="X14" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="Y14" s="11"/>
-      <c r="Z14" s="11"/>
-      <c r="AA14" s="11"/>
-      <c r="AB14" s="11"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="10"/>
+      <c r="AA14" s="10"/>
+      <c r="AB14" s="10"/>
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
     </row>
     <row r="15" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="9" t="str">
-        <f t="shared" ref="L15:X15" si="2">IF(L42=0,"",IF(L42&gt;1,"❷","①"))</f>
-        <v/>
-      </c>
-      <c r="M15" s="9" t="str">
+      <c r="C15" s="15"/>
+      <c r="D15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="8" t="str">
+        <f t="shared" ref="L15:W15" si="2">IF(L42=0,"",IF(L42&gt;1,"❷","①"))</f>
+        <v/>
+      </c>
+      <c r="M15" s="8" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="N15" s="9" t="str">
+      <c r="N15" s="8" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="O15" s="9" t="str">
+      <c r="O15" s="8" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="P15" s="9" t="str">
+      <c r="P15" s="8" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="Q15" s="9" t="str">
+      <c r="Q15" s="8" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="R15" s="9" t="str">
+      <c r="R15" s="8" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="S15" s="9" t="str">
+      <c r="S15" s="8" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="T15" s="9" t="str">
+      <c r="T15" s="8" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="U15" s="9" t="str">
+      <c r="U15" s="8" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="V15" s="9" t="str">
+      <c r="V15" s="8" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="W15" s="9" t="str">
+      <c r="W15" s="8" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="X15" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="Y15" s="11"/>
-      <c r="Z15" s="11"/>
-      <c r="AA15" s="11"/>
-      <c r="AB15" s="11"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="10"/>
+      <c r="AA15" s="10"/>
+      <c r="AB15" s="10"/>
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
     </row>
     <row r="16" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="9" t="str">
-        <f t="shared" ref="L16:X16" si="3">IF(L43=0,"",IF(L43&gt;1,"❷","①"))</f>
-        <v/>
-      </c>
-      <c r="M16" s="9" t="str">
+      <c r="C16" s="15"/>
+      <c r="D16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="8" t="str">
+        <f t="shared" ref="L16:W16" si="3">IF(L43=0,"",IF(L43&gt;1,"❷","①"))</f>
+        <v/>
+      </c>
+      <c r="M16" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="N16" s="9" t="str">
+      <c r="N16" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="O16" s="9" t="str">
+      <c r="O16" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="P16" s="9" t="str">
+      <c r="P16" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="Q16" s="9" t="str">
+      <c r="Q16" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="R16" s="9" t="str">
+      <c r="R16" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="S16" s="9" t="str">
+      <c r="S16" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="T16" s="9" t="str">
+      <c r="T16" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="U16" s="9" t="str">
+      <c r="U16" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="V16" s="9" t="str">
+      <c r="V16" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W16" s="9" t="str">
+      <c r="W16" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="X16" s="9" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="Y16" s="11"/>
-      <c r="Z16" s="11"/>
-      <c r="AA16" s="11"/>
-      <c r="AB16" s="11"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="10"/>
+      <c r="AB16" s="10"/>
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
     </row>
     <row r="17" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="9" t="str">
-        <f t="shared" ref="L17:X17" si="4">IF(L44=0,"",IF(L44&gt;1,"❷","①"))</f>
-        <v/>
-      </c>
-      <c r="M17" s="9" t="str">
+      <c r="C17" s="15"/>
+      <c r="D17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="8" t="str">
+        <f t="shared" ref="L17:W17" si="4">IF(L44=0,"",IF(L44&gt;1,"❷","①"))</f>
+        <v/>
+      </c>
+      <c r="M17" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="N17" s="9" t="str">
+      <c r="N17" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="O17" s="9" t="str">
+      <c r="O17" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="P17" s="9" t="str">
+      <c r="P17" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="Q17" s="9" t="str">
+      <c r="Q17" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="R17" s="9" t="str">
+      <c r="R17" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="S17" s="9" t="str">
+      <c r="S17" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="T17" s="9" t="str">
+      <c r="T17" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="U17" s="9" t="str">
+      <c r="U17" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="V17" s="9" t="str">
+      <c r="V17" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="W17" s="9" t="str">
+      <c r="W17" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="X17" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="Y17" s="11"/>
-      <c r="Z17" s="11"/>
-      <c r="AA17" s="11"/>
-      <c r="AB17" s="11"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="10"/>
+      <c r="AA17" s="10"/>
+      <c r="AB17" s="10"/>
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
     </row>
     <row r="18" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="9" t="str">
-        <f t="shared" ref="L18:X18" si="5">IF(L45=0,"",IF(L45&gt;1,"❷","①"))</f>
-        <v/>
-      </c>
-      <c r="M18" s="9" t="str">
+      <c r="C18" s="15"/>
+      <c r="D18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="8" t="str">
+        <f t="shared" ref="L18:W18" si="5">IF(L45=0,"",IF(L45&gt;1,"❷","①"))</f>
+        <v/>
+      </c>
+      <c r="M18" s="8" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="N18" s="9" t="str">
+      <c r="N18" s="8" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="O18" s="9" t="str">
+      <c r="O18" s="8" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="P18" s="9" t="str">
+      <c r="P18" s="8" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="Q18" s="9" t="str">
+      <c r="Q18" s="8" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="R18" s="9" t="str">
+      <c r="R18" s="8" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="S18" s="9" t="str">
+      <c r="S18" s="8" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="T18" s="9" t="str">
+      <c r="T18" s="8" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="U18" s="9" t="str">
+      <c r="U18" s="8" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="V18" s="9" t="str">
+      <c r="V18" s="8" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="W18" s="9" t="str">
+      <c r="W18" s="8" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="X18" s="9" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Y18" s="11"/>
-      <c r="Z18" s="11"/>
-      <c r="AA18" s="11"/>
-      <c r="AB18" s="11"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="10"/>
+      <c r="AA18" s="10"/>
+      <c r="AB18" s="10"/>
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
     </row>
     <row r="19" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="9" t="str">
-        <f t="shared" ref="L19:X19" si="6">IF(L46=0,"",IF(L46&gt;1,"❷","①"))</f>
-        <v/>
-      </c>
-      <c r="M19" s="9" t="str">
+      <c r="C19" s="15"/>
+      <c r="D19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="8" t="str">
+        <f t="shared" ref="L19:W19" si="6">IF(L46=0,"",IF(L46&gt;1,"❷","①"))</f>
+        <v/>
+      </c>
+      <c r="M19" s="8" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="N19" s="9" t="str">
+      <c r="N19" s="8" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="O19" s="9" t="str">
+      <c r="O19" s="8" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="P19" s="9" t="str">
+      <c r="P19" s="8" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="Q19" s="9" t="str">
+      <c r="Q19" s="8" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="R19" s="9" t="str">
+      <c r="R19" s="8" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="S19" s="9" t="str">
+      <c r="S19" s="8" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="T19" s="9" t="str">
+      <c r="T19" s="8" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="U19" s="9" t="str">
+      <c r="U19" s="8" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="V19" s="9" t="str">
+      <c r="V19" s="8" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="W19" s="9" t="str">
+      <c r="W19" s="8" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="X19" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="Y19" s="11"/>
-      <c r="Z19" s="11"/>
-      <c r="AA19" s="11"/>
-      <c r="AB19" s="11"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="10"/>
+      <c r="AA19" s="10"/>
+      <c r="AB19" s="10"/>
       <c r="AC19" s="1"/>
       <c r="AD19" s="1"/>
     </row>
     <row r="20" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="19" t="s">
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
+      <c r="U20" s="14"/>
+      <c r="V20" s="17"/>
+      <c r="W20" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
-      <c r="Q20" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="R20" s="17"/>
-      <c r="S20" s="17"/>
-      <c r="T20" s="17"/>
-      <c r="U20" s="17"/>
-      <c r="V20" s="20"/>
-      <c r="W20" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="X20" s="22"/>
-      <c r="Y20" s="22"/>
-      <c r="Z20" s="22"/>
-      <c r="AA20" s="22"/>
-      <c r="AB20" s="23"/>
+      <c r="X20" s="19"/>
+      <c r="Y20" s="19"/>
+      <c r="Z20" s="19"/>
+      <c r="AA20" s="19"/>
+      <c r="AB20" s="20"/>
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
     </row>
     <row r="21" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="10"/>
+      <c r="D21" s="9"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -1955,70 +1936,70 @@
       <c r="AD21" s="1"/>
     </row>
     <row r="22" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B22" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="15"/>
-      <c r="T22" s="15"/>
-      <c r="U22" s="15"/>
-      <c r="V22" s="15"/>
-      <c r="W22" s="15"/>
-      <c r="X22" s="15"/>
-      <c r="Y22" s="15"/>
-      <c r="Z22" s="15"/>
-      <c r="AA22" s="15"/>
-      <c r="AB22" s="15"/>
-      <c r="AC22" s="15"/>
-      <c r="AD22" s="15"/>
+      <c r="B22" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="12"/>
+      <c r="V22" s="12"/>
+      <c r="W22" s="12"/>
+      <c r="X22" s="12"/>
+      <c r="Y22" s="12"/>
+      <c r="Z22" s="12"/>
+      <c r="AA22" s="12"/>
+      <c r="AB22" s="12"/>
+      <c r="AC22" s="12"/>
+      <c r="AD22" s="12"/>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="15" t="s">
+      <c r="B23" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
-      <c r="T23" s="15"/>
-      <c r="U23" s="15"/>
-      <c r="V23" s="15"/>
-      <c r="W23" s="15"/>
-      <c r="X23" s="15"/>
-      <c r="Y23" s="15"/>
-      <c r="Z23" s="15"/>
-      <c r="AA23" s="15"/>
-      <c r="AB23" s="15"/>
-      <c r="AC23" s="1"/>
-      <c r="AD23" s="1"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
+      <c r="T23" s="12"/>
+      <c r="U23" s="12"/>
+      <c r="V23" s="12"/>
+      <c r="W23" s="12"/>
+      <c r="X23" s="12"/>
+      <c r="Y23" s="12"/>
+      <c r="Z23" s="12"/>
+      <c r="AA23" s="12"/>
+      <c r="AB23" s="12"/>
+      <c r="AC23" s="12"/>
+      <c r="AD23" s="12"/>
     </row>
     <row r="24" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
@@ -2053,7 +2034,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D23:AB23"/>
+    <mergeCell ref="D2:AB2"/>
+    <mergeCell ref="B7:AD7"/>
+    <mergeCell ref="B8:AD8"/>
+    <mergeCell ref="D9:AB9"/>
+    <mergeCell ref="B5:AD5"/>
     <mergeCell ref="B4:AD4"/>
     <mergeCell ref="B22:AD22"/>
     <mergeCell ref="E11:AB11"/>
@@ -2062,11 +2047,7 @@
     <mergeCell ref="K20:P20"/>
     <mergeCell ref="Q20:V20"/>
     <mergeCell ref="W20:AB20"/>
-    <mergeCell ref="D2:AB2"/>
-    <mergeCell ref="D5:AB5"/>
-    <mergeCell ref="B7:AD7"/>
-    <mergeCell ref="B8:AD8"/>
-    <mergeCell ref="D9:AB9"/>
+    <mergeCell ref="B23:AD23"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:AB19">
     <cfRule type="colorScale" priority="1">

</xml_diff>